<commit_message>
refactor(rename): rename files and added recruit_age again
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_non_repeated.xlsx
+++ b/R/data/dictionaries/1_0/1_0_non_repeated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9758439D-5F07-DF4F-B003-DEFAF647C37D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D427E4F4-0B90-1E46-AFCD-E9F44F587524}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="463">
   <si>
     <t>name</t>
   </si>
@@ -1404,13 +1404,19 @@
   </si>
   <si>
     <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>recruit_age</t>
+  </si>
+  <si>
+    <t>Age of the child at time of enrolment. In days. Negative if prepartum, positive if postpartum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1436,6 +1442,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1445,7 +1457,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1468,13 +1480,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1485,6 +1508,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1948,10 +1974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG109"/>
+  <dimension ref="A1:BG110"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1959,7 +1985,7 @@
     <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="73" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -3645,6 +3671,20 @@
         <v>424</v>
       </c>
     </row>
+    <row r="110" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>462</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="2048"/>
@@ -3658,7 +3698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D472"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>